<commit_message>
built unigram dictionary and saved to rdata
</commit_message>
<xml_diff>
--- a/2_code/2_sentiment_analysis/1_basic_unigram_dict/dicts/list-sources.xlsx
+++ b/2_code/2_sentiment_analysis/1_basic_unigram_dict/dicts/list-sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\consulting\projects\consulting\2_code\2_sentiment_analysis\1_basic_unigram_dict\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8869FADE-E607-417F-83DE-F2B936FCB25A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ADC914-306A-4857-A0B6-83722A45E6BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A97FC25-B009-4150-BADE-91670A5B071B}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>dictionary</t>
   </si>
   <si>
-    <t>dissertation (über paul thurner)</t>
-  </si>
-  <si>
     <t>SentiWS*</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>https://github.com/stopwords-iso/stopwords-de</t>
+  </si>
+  <si>
+    <t>http://www.ulliwaltinger.de/sentiment/</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,40 +459,40 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>